<commit_message>
Clean t28 & Res t10
</commit_message>
<xml_diff>
--- a/5_Analysis/Label.xlsx
+++ b/5_Analysis/Label.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\YuKi_Project\Self\yuki_Reliability_SPMT\5_Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BAE99DC-314A-4B33-92DE-5F06972A2A0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58E60CE3-3734-49A1-96F9-3AC5BBE25AB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-105" yWindow="0" windowWidth="19410" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="136">
   <si>
     <t>Paper_ID</t>
   </si>
@@ -792,6 +792,43 @@
   </si>
   <si>
     <t>Conditon: (Self, Stranger)</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pt28E1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Amodeo et al.</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>ASD: (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Non</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>; ASD)</t>
+    </r>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1793,12 +1830,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S44"/>
+  <dimension ref="A1:S45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="topRight" activeCell="D43" sqref="D43"/>
+      <selection pane="topRight" activeCell="R46" sqref="R46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1958,7 +1995,7 @@
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
       <c r="N3" s="1">
-        <f t="shared" ref="N3:N44" si="0">J3-L3-M3</f>
+        <f t="shared" ref="N3:N45" si="0">J3-L3-M3</f>
         <v>46</v>
       </c>
       <c r="O3" s="1" t="s">
@@ -3760,6 +3797,48 @@
       </c>
       <c r="R44" t="s">
         <v>132</v>
+      </c>
+    </row>
+    <row r="45" spans="1:18" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B45">
+        <v>44</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="D45" s="1">
+        <v>1</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H45" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J45" s="1">
+        <v>30</v>
+      </c>
+      <c r="K45" s="1">
+        <v>60</v>
+      </c>
+      <c r="N45" s="1">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="O45" t="s">
+        <v>134</v>
+      </c>
+      <c r="P45" s="1">
+        <v>2024</v>
+      </c>
+      <c r="Q45">
+        <v>1</v>
+      </c>
+      <c r="R45" t="s">
+        <v>135</v>
       </c>
     </row>
   </sheetData>

</xml_diff>